<commit_message>
Change in schema. Now we have ObsEntities instead of plant_parts. Added tons of tests in models css changed
</commit_message>
<xml_diff>
--- a/vavilov/test/data/traits.xlsx
+++ b/vavilov/test/data/traits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">grow habit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area defined by the outer bounday of the fruit measured in the longitudinal section</t>
   </si>
 </sst>
 </file>
@@ -47,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -68,6 +74,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,8 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,24 +151,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.75"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -174,6 +190,17 @@
       </c>
       <c r="C2" s="0" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change all views with images to use new json based galleria data provider
</commit_message>
<xml_diff>
--- a/vavilov/test/data/traits.xlsx
+++ b/vavilov/test/data/traits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -44,6 +44,15 @@
   </si>
   <si>
     <t xml:space="preserve">Area defined by the outer bounday of the fruit measured in the longitudinal section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_leaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaf image</t>
   </si>
 </sst>
 </file>
@@ -151,23 +160,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,6 +211,17 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added related observation load functions
</commit_message>
<xml_diff>
--- a/vavilov/test/data/traits.xlsx
+++ b/vavilov/test/data/traits.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -53,6 +53,33 @@
   </si>
   <si>
     <t xml:space="preserve">leaf image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAB Color1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAB_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAB Color2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAB Color3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAB Color4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number_fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verage_Fruit_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average_Fruit_weight_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fruit_weight_g</t>
   </si>
 </sst>
 </file>
@@ -160,22 +187,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
@@ -222,6 +249,70 @@
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>